<commit_message>
update AFCON xlsx file
</commit_message>
<xml_diff>
--- a/src/data/AFCON-2023.xlsx
+++ b/src/data/AFCON-2023.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2361" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2363" uniqueCount="398">
   <si>
     <t>Group</t>
   </si>
@@ -1325,6 +1325,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFF2CC"/>
         <bgColor rgb="FFFFF2CC"/>
       </patternFill>
@@ -1339,12 +1345,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFA2C4C9"/>
         <bgColor rgb="FFA2C4C9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor theme="7"/>
       </patternFill>
     </fill>
     <fill>
@@ -1392,7 +1392,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="55">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1474,12 +1474,6 @@
     <xf borderId="1" fillId="13" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="1" fillId="14" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -1498,6 +1492,15 @@
     <xf borderId="1" fillId="16" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="1" fillId="17" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="17" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -1508,14 +1511,11 @@
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="17" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="17" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="14" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="12" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="18" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="1" fillId="15" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="16" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="6" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="19" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
@@ -1538,9 +1538,6 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="21" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="17" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -13453,6 +13450,84 @@
       <c r="E104" s="27" t="s">
         <v>24</v>
       </c>
+      <c r="F104" s="27">
+        <v>37.6</v>
+      </c>
+      <c r="G104" s="27">
+        <v>40.8</v>
+      </c>
+      <c r="H104" s="27">
+        <v>37.9</v>
+      </c>
+      <c r="I104" s="27">
+        <v>3.0</v>
+      </c>
+      <c r="J104" s="27">
+        <v>0.0</v>
+      </c>
+      <c r="K104" s="27">
+        <v>4.0</v>
+      </c>
+      <c r="L104" s="27">
+        <v>249.0</v>
+      </c>
+      <c r="M104" s="27">
+        <v>52.0</v>
+      </c>
+      <c r="N104" s="27">
+        <v>74.3</v>
+      </c>
+      <c r="O104" s="27">
+        <v>54.9</v>
+      </c>
+      <c r="P104" s="27">
+        <v>15.0</v>
+      </c>
+      <c r="Q104" s="27">
+        <v>13.3</v>
+      </c>
+      <c r="R104" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="S104" s="27">
+        <v>5.0</v>
+      </c>
+      <c r="T104" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="U104" s="27">
+        <v>2.0</v>
+      </c>
+      <c r="V104" s="27">
+        <v>1.0</v>
+      </c>
+      <c r="W104" s="27">
+        <v>4.0</v>
+      </c>
+      <c r="X104" s="27">
+        <v>20.0</v>
+      </c>
+      <c r="Y104" s="27">
+        <v>13.0</v>
+      </c>
+      <c r="Z104" s="27">
+        <v>69.2</v>
+      </c>
+      <c r="AA104" s="27">
+        <v>30.0</v>
+      </c>
+      <c r="AB104" s="27">
+        <v>18.0</v>
+      </c>
+      <c r="AC104" s="27">
+        <v>2.0</v>
+      </c>
+      <c r="AD104" s="27">
+        <v>0.0</v>
+      </c>
+      <c r="AE104" s="27" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="27" t="s">
@@ -13469,6 +13544,84 @@
       </c>
       <c r="E105" s="27" t="s">
         <v>11</v>
+      </c>
+      <c r="F105" s="27">
+        <v>62.4</v>
+      </c>
+      <c r="G105" s="27">
+        <v>59.2</v>
+      </c>
+      <c r="H105" s="27">
+        <v>62.1</v>
+      </c>
+      <c r="I105" s="27">
+        <v>4.0</v>
+      </c>
+      <c r="J105" s="27">
+        <v>0.0</v>
+      </c>
+      <c r="K105" s="27">
+        <v>6.0</v>
+      </c>
+      <c r="L105" s="27">
+        <v>410.0</v>
+      </c>
+      <c r="M105" s="27">
+        <v>35.0</v>
+      </c>
+      <c r="N105" s="27">
+        <v>86.6</v>
+      </c>
+      <c r="O105" s="27">
+        <v>73.3</v>
+      </c>
+      <c r="P105" s="27">
+        <v>29.0</v>
+      </c>
+      <c r="Q105" s="27">
+        <v>24.1</v>
+      </c>
+      <c r="R105" s="27">
+        <v>2.0</v>
+      </c>
+      <c r="S105" s="27">
+        <v>18.0</v>
+      </c>
+      <c r="T105" s="27">
+        <v>8.0</v>
+      </c>
+      <c r="U105" s="27">
+        <v>2.0</v>
+      </c>
+      <c r="V105" s="27">
+        <v>5.0</v>
+      </c>
+      <c r="W105" s="27">
+        <v>13.0</v>
+      </c>
+      <c r="X105" s="27">
+        <v>44.4</v>
+      </c>
+      <c r="Y105" s="27">
+        <v>15.0</v>
+      </c>
+      <c r="Z105" s="27">
+        <v>46.7</v>
+      </c>
+      <c r="AA105" s="27">
+        <v>25.0</v>
+      </c>
+      <c r="AB105" s="27">
+        <v>15.0</v>
+      </c>
+      <c r="AC105" s="27">
+        <v>3.0</v>
+      </c>
+      <c r="AD105" s="27">
+        <v>0.0</v>
+      </c>
+      <c r="AE105" s="27" t="s">
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -15618,7 +15771,7 @@
       </c>
     </row>
     <row r="107">
-      <c r="B107" s="28"/>
+      <c r="B107" s="35"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -15665,2801 +15818,2801 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="36" t="s">
         <v>214</v>
       </c>
-      <c r="B2" s="36">
+      <c r="B2" s="37">
         <v>45304.0</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="G2" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="H2" s="37">
+      <c r="F2" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="G2" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="H2" s="38">
         <f t="shared" ref="H2:H105" si="1">$F2-$G2</f>
         <v>2</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="36" t="s">
         <v>214</v>
       </c>
-      <c r="B3" s="36">
+      <c r="B3" s="37">
         <v>45304.0</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="G3" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="H3" s="37">
+      <c r="F3" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="G3" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="H3" s="38">
         <f t="shared" si="1"/>
         <v>-2</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="36" t="s">
         <v>217</v>
       </c>
-      <c r="B4" s="36">
+      <c r="B4" s="37">
         <v>45305.0</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="G4" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="H4" s="37">
+      <c r="F4" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="G4" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="H4" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="36" t="s">
         <v>217</v>
       </c>
-      <c r="B5" s="36">
+      <c r="B5" s="37">
         <v>45305.0</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="G5" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="H5" s="37">
+      <c r="F5" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="G5" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="H5" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="36" t="s">
         <v>217</v>
       </c>
-      <c r="B6" s="36">
+      <c r="B6" s="37">
         <v>45305.0</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="35" t="s">
+      <c r="E6" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="G6" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="H6" s="37">
+      <c r="F6" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="G6" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="H6" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="36" t="s">
         <v>217</v>
       </c>
-      <c r="B7" s="36">
+      <c r="B7" s="37">
         <v>45305.0</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="35" t="s">
+      <c r="E7" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="G7" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="H7" s="37">
+      <c r="F7" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="G7" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="H7" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="36" t="s">
         <v>217</v>
       </c>
-      <c r="B8" s="36">
+      <c r="B8" s="37">
         <v>45305.0</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="35" t="s">
+      <c r="E8" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="G8" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="H8" s="37">
+      <c r="F8" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="G8" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="H8" s="38">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="36" t="s">
         <v>217</v>
       </c>
-      <c r="B9" s="36">
+      <c r="B9" s="37">
         <v>45305.0</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="D9" s="35" t="s">
+      <c r="D9" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="35" t="s">
+      <c r="E9" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="F9" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="G9" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="H9" s="37">
+      <c r="F9" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="G9" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="H9" s="38">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="36" t="s">
         <v>219</v>
       </c>
-      <c r="B10" s="36">
+      <c r="B10" s="37">
         <v>45306.0</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="D10" s="35" t="s">
+      <c r="D10" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="E10" s="35" t="s">
+      <c r="E10" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="F10" s="35">
+      <c r="F10" s="36">
         <v>3.0</v>
       </c>
-      <c r="G10" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="H10" s="37">
+      <c r="G10" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="H10" s="38">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="36" t="s">
         <v>219</v>
       </c>
-      <c r="B11" s="36">
+      <c r="B11" s="37">
         <v>45306.0</v>
       </c>
-      <c r="C11" s="35" t="s">
+      <c r="C11" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="D11" s="35" t="s">
+      <c r="D11" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="E11" s="35" t="s">
+      <c r="E11" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="F11" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="G11" s="35">
+      <c r="F11" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="G11" s="36">
         <v>3.0</v>
       </c>
-      <c r="H11" s="37">
+      <c r="H11" s="38">
         <f t="shared" si="1"/>
         <v>-3</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="36" t="s">
         <v>219</v>
       </c>
-      <c r="B12" s="36">
+      <c r="B12" s="37">
         <v>45306.0</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="E12" s="35" t="s">
+      <c r="E12" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="F12" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="G12" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="H12" s="37">
+      <c r="F12" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="G12" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="H12" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="36" t="s">
         <v>219</v>
       </c>
-      <c r="B13" s="36">
+      <c r="B13" s="37">
         <v>45306.0</v>
       </c>
-      <c r="C13" s="35" t="s">
+      <c r="C13" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="D13" s="35" t="s">
+      <c r="D13" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="35" t="s">
+      <c r="E13" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="F13" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="G13" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="H13" s="37">
+      <c r="F13" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="G13" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="H13" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="35" t="s">
+      <c r="A14" s="36" t="s">
         <v>219</v>
       </c>
-      <c r="B14" s="36">
+      <c r="B14" s="37">
         <v>45306.0</v>
       </c>
-      <c r="C14" s="35" t="s">
+      <c r="C14" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="D14" s="35" t="s">
+      <c r="D14" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="E14" s="35" t="s">
+      <c r="E14" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="F14" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="G14" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="H14" s="37">
+      <c r="F14" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="G14" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="H14" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="36" t="s">
         <v>219</v>
       </c>
-      <c r="B15" s="36">
+      <c r="B15" s="37">
         <v>45306.0</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="D15" s="35" t="s">
+      <c r="D15" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="E15" s="35" t="s">
+      <c r="E15" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="F15" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="G15" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="H15" s="37">
+      <c r="F15" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="G15" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="H15" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="B16" s="36">
+      <c r="B16" s="37">
         <v>45307.0</v>
       </c>
-      <c r="C16" s="35" t="s">
+      <c r="C16" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="D16" s="35" t="s">
+      <c r="D16" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="E16" s="35" t="s">
+      <c r="E16" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="F16" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="G16" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="H16" s="37">
+      <c r="F16" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="G16" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="H16" s="38">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="B17" s="36">
+      <c r="B17" s="37">
         <v>45307.0</v>
       </c>
-      <c r="C17" s="35" t="s">
+      <c r="C17" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="D17" s="35" t="s">
+      <c r="D17" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="E17" s="35" t="s">
+      <c r="E17" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="F17" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="G17" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="H17" s="37">
+      <c r="F17" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="G17" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="H17" s="38">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="B18" s="36">
+      <c r="B18" s="37">
         <v>45307.0</v>
       </c>
-      <c r="C18" s="35" t="s">
+      <c r="C18" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="D18" s="35" t="s">
+      <c r="D18" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="E18" s="35" t="s">
+      <c r="E18" s="36" t="s">
         <v>115</v>
       </c>
-      <c r="F18" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="G18" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="H18" s="37">
+      <c r="F18" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="G18" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="H18" s="38">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="B19" s="36">
+      <c r="B19" s="37">
         <v>45307.0</v>
       </c>
-      <c r="C19" s="35" t="s">
+      <c r="C19" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="D19" s="35" t="s">
+      <c r="D19" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="E19" s="35" t="s">
+      <c r="E19" s="36" t="s">
         <v>121</v>
       </c>
-      <c r="F19" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="G19" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="H19" s="37">
+      <c r="F19" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="G19" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="H19" s="38">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="35" t="s">
+      <c r="A20" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="B20" s="36">
+      <c r="B20" s="37">
         <v>45307.0</v>
       </c>
-      <c r="C20" s="35" t="s">
+      <c r="C20" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="D20" s="35" t="s">
+      <c r="D20" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="E20" s="35" t="s">
+      <c r="E20" s="36" t="s">
         <v>127</v>
       </c>
-      <c r="F20" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="G20" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="H20" s="37">
+      <c r="F20" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="G20" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="H20" s="38">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="35" t="s">
+      <c r="A21" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="B21" s="36">
+      <c r="B21" s="37">
         <v>45307.0</v>
       </c>
-      <c r="C21" s="35" t="s">
+      <c r="C21" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="D21" s="35" t="s">
+      <c r="D21" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="E21" s="35" t="s">
+      <c r="E21" s="36" t="s">
         <v>133</v>
       </c>
-      <c r="F21" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="G21" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="H21" s="37">
+      <c r="F21" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="G21" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="H21" s="38">
         <f t="shared" si="1"/>
         <v>-2</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="35" t="s">
+      <c r="A22" s="36" t="s">
         <v>221</v>
       </c>
-      <c r="B22" s="36">
+      <c r="B22" s="37">
         <v>45308.0</v>
       </c>
-      <c r="C22" s="35" t="s">
+      <c r="C22" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="D22" s="35" t="s">
+      <c r="D22" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="E22" s="35" t="s">
+      <c r="E22" s="36" t="s">
         <v>140</v>
       </c>
-      <c r="F22" s="35">
+      <c r="F22" s="36">
         <v>3.0</v>
       </c>
-      <c r="G22" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="H22" s="37">
+      <c r="G22" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="H22" s="38">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="35" t="s">
+      <c r="A23" s="36" t="s">
         <v>221</v>
       </c>
-      <c r="B23" s="36">
+      <c r="B23" s="37">
         <v>45308.0</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="D23" s="35" t="s">
+      <c r="D23" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="E23" s="35" t="s">
+      <c r="E23" s="36" t="s">
         <v>146</v>
       </c>
-      <c r="F23" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="G23" s="35">
+      <c r="F23" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="G23" s="36">
         <v>3.0</v>
       </c>
-      <c r="H23" s="37">
+      <c r="H23" s="38">
         <f t="shared" si="1"/>
         <v>-3</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="35" t="s">
+      <c r="A24" s="36" t="s">
         <v>221</v>
       </c>
-      <c r="B24" s="36">
+      <c r="B24" s="37">
         <v>45308.0</v>
       </c>
-      <c r="C24" s="35" t="s">
+      <c r="C24" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="D24" s="35" t="s">
+      <c r="D24" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="E24" s="35" t="s">
+      <c r="E24" s="36" t="s">
         <v>153</v>
       </c>
-      <c r="F24" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="G24" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="H24" s="37">
+      <c r="F24" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="G24" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="H24" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="35" t="s">
+      <c r="A25" s="36" t="s">
         <v>221</v>
       </c>
-      <c r="B25" s="36">
+      <c r="B25" s="37">
         <v>45308.0</v>
       </c>
-      <c r="C25" s="35" t="s">
+      <c r="C25" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="D25" s="35" t="s">
+      <c r="D25" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="E25" s="35" t="s">
+      <c r="E25" s="36" t="s">
         <v>159</v>
       </c>
-      <c r="F25" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="G25" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="H25" s="37">
+      <c r="F25" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="G25" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="H25" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="35" t="s">
+      <c r="A26" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="B26" s="36">
+      <c r="B26" s="37">
         <v>45309.0</v>
       </c>
-      <c r="C26" s="35" t="s">
+      <c r="C26" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="D26" s="35" t="s">
+      <c r="D26" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="E26" s="35" t="s">
+      <c r="E26" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="F26" s="35">
+      <c r="F26" s="36">
         <v>4.0</v>
       </c>
-      <c r="G26" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="H26" s="37">
+      <c r="G26" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="H26" s="38">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="35" t="s">
+      <c r="A27" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="B27" s="36">
+      <c r="B27" s="37">
         <v>45309.0</v>
       </c>
-      <c r="C27" s="35" t="s">
+      <c r="C27" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="D27" s="35" t="s">
+      <c r="D27" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="E27" s="35" t="s">
+      <c r="E27" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="F27" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="G27" s="35">
+      <c r="F27" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="G27" s="36">
         <v>4.0</v>
       </c>
-      <c r="H27" s="37">
+      <c r="H27" s="38">
         <f t="shared" si="1"/>
         <v>-2</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="35" t="s">
+      <c r="A28" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="B28" s="36">
+      <c r="B28" s="37">
         <v>45309.0</v>
       </c>
-      <c r="C28" s="35" t="s">
+      <c r="C28" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="D28" s="35" t="s">
+      <c r="D28" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="E28" s="35" t="s">
+      <c r="E28" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="F28" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="G28" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="H28" s="37">
+      <c r="F28" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="G28" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="H28" s="38">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="B29" s="36">
+      <c r="B29" s="37">
         <v>45309.0</v>
       </c>
-      <c r="C29" s="35" t="s">
+      <c r="C29" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="D29" s="35" t="s">
+      <c r="D29" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="E29" s="35" t="s">
+      <c r="E29" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="F29" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="G29" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="H29" s="37">
+      <c r="F29" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="G29" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="H29" s="38">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="35" t="s">
+      <c r="A30" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="B30" s="36">
+      <c r="B30" s="37">
         <v>45309.0</v>
       </c>
-      <c r="C30" s="35" t="s">
+      <c r="C30" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="D30" s="35" t="s">
+      <c r="D30" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="E30" s="35" t="s">
+      <c r="E30" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="F30" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="G30" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="H30" s="37">
+      <c r="F30" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="G30" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="H30" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="35" t="s">
+      <c r="A31" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="B31" s="36">
+      <c r="B31" s="37">
         <v>45309.0</v>
       </c>
-      <c r="C31" s="35" t="s">
+      <c r="C31" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="D31" s="35" t="s">
+      <c r="D31" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="E31" s="35" t="s">
+      <c r="E31" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="F31" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="G31" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="H31" s="37">
+      <c r="F31" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="G31" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="H31" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="35" t="s">
+      <c r="A32" s="36" t="s">
         <v>223</v>
       </c>
-      <c r="B32" s="36">
+      <c r="B32" s="37">
         <v>45310.0</v>
       </c>
-      <c r="C32" s="35" t="s">
+      <c r="C32" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="D32" s="35" t="s">
+      <c r="D32" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="E32" s="35" t="s">
+      <c r="E32" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="F32" s="35">
+      <c r="F32" s="36">
         <v>3.0</v>
       </c>
-      <c r="G32" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="H32" s="37">
+      <c r="G32" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="H32" s="38">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="35" t="s">
+      <c r="A33" s="36" t="s">
         <v>223</v>
       </c>
-      <c r="B33" s="36">
+      <c r="B33" s="37">
         <v>45310.0</v>
       </c>
-      <c r="C33" s="35" t="s">
+      <c r="C33" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="D33" s="35" t="s">
+      <c r="D33" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="E33" s="35" t="s">
+      <c r="E33" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="F33" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="G33" s="35">
+      <c r="F33" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="G33" s="36">
         <v>3.0</v>
       </c>
-      <c r="H33" s="37">
+      <c r="H33" s="38">
         <f t="shared" si="1"/>
         <v>-3</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="35" t="s">
+      <c r="A34" s="36" t="s">
         <v>223</v>
       </c>
-      <c r="B34" s="36">
+      <c r="B34" s="37">
         <v>45310.0</v>
       </c>
-      <c r="C34" s="35" t="s">
+      <c r="C34" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="D34" s="35" t="s">
+      <c r="D34" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="E34" s="35" t="s">
+      <c r="E34" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="F34" s="35">
+      <c r="F34" s="36">
         <v>3.0</v>
       </c>
-      <c r="G34" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="H34" s="37">
+      <c r="G34" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="H34" s="38">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="35" t="s">
+      <c r="A35" s="36" t="s">
         <v>223</v>
       </c>
-      <c r="B35" s="36">
+      <c r="B35" s="37">
         <v>45310.0</v>
       </c>
-      <c r="C35" s="35" t="s">
+      <c r="C35" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="D35" s="35" t="s">
+      <c r="D35" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="E35" s="35" t="s">
+      <c r="E35" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="F35" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="G35" s="35">
+      <c r="F35" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="G35" s="36">
         <v>3.0</v>
       </c>
-      <c r="H35" s="37">
+      <c r="H35" s="38">
         <f t="shared" si="1"/>
         <v>-2</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="35" t="s">
+      <c r="A36" s="36" t="s">
         <v>223</v>
       </c>
-      <c r="B36" s="36">
+      <c r="B36" s="37">
         <v>45310.0</v>
       </c>
-      <c r="C36" s="35" t="s">
+      <c r="C36" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="D36" s="35" t="s">
+      <c r="D36" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="E36" s="35" t="s">
+      <c r="E36" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="F36" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="G36" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="H36" s="37">
+      <c r="F36" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="G36" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="H36" s="38">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="35" t="s">
+      <c r="A37" s="36" t="s">
         <v>223</v>
       </c>
-      <c r="B37" s="36">
+      <c r="B37" s="37">
         <v>45310.0</v>
       </c>
-      <c r="C37" s="35" t="s">
+      <c r="C37" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="D37" s="35" t="s">
+      <c r="D37" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="E37" s="35" t="s">
+      <c r="E37" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="F37" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="G37" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="H37" s="37">
+      <c r="F37" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="G37" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="H37" s="38">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="35" t="s">
+      <c r="A38" s="36" t="s">
         <v>224</v>
       </c>
-      <c r="B38" s="36">
+      <c r="B38" s="37">
         <v>45311.0</v>
       </c>
-      <c r="C38" s="35" t="s">
+      <c r="C38" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="D38" s="35" t="s">
+      <c r="D38" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="E38" s="35" t="s">
+      <c r="E38" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="F38" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="G38" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="H38" s="37">
+      <c r="F38" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="G38" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="H38" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="35" t="s">
+      <c r="A39" s="36" t="s">
         <v>224</v>
       </c>
-      <c r="B39" s="36">
+      <c r="B39" s="37">
         <v>45311.0</v>
       </c>
-      <c r="C39" s="35" t="s">
+      <c r="C39" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="D39" s="35" t="s">
+      <c r="D39" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="E39" s="35" t="s">
+      <c r="E39" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="F39" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="G39" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="H39" s="37">
+      <c r="F39" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="G39" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="H39" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="35" t="s">
+      <c r="A40" s="36" t="s">
         <v>224</v>
       </c>
-      <c r="B40" s="36">
+      <c r="B40" s="37">
         <v>45311.0</v>
       </c>
-      <c r="C40" s="35" t="s">
+      <c r="C40" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="D40" s="35" t="s">
+      <c r="D40" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="E40" s="35" t="s">
+      <c r="E40" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="F40" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="G40" s="35">
+      <c r="F40" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="G40" s="36">
         <v>3.0</v>
       </c>
-      <c r="H40" s="37">
+      <c r="H40" s="38">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="35" t="s">
+      <c r="A41" s="36" t="s">
         <v>224</v>
       </c>
-      <c r="B41" s="36">
+      <c r="B41" s="37">
         <v>45311.0</v>
       </c>
-      <c r="C41" s="35" t="s">
+      <c r="C41" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="D41" s="35" t="s">
+      <c r="D41" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="E41" s="35" t="s">
+      <c r="E41" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="F41" s="35">
+      <c r="F41" s="36">
         <v>3.0</v>
       </c>
-      <c r="G41" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="H41" s="37">
+      <c r="G41" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="H41" s="38">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="35" t="s">
+      <c r="A42" s="36" t="s">
         <v>224</v>
       </c>
-      <c r="B42" s="36">
+      <c r="B42" s="37">
         <v>45311.0</v>
       </c>
-      <c r="C42" s="35" t="s">
+      <c r="C42" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="D42" s="35" t="s">
+      <c r="D42" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="E42" s="35" t="s">
+      <c r="E42" s="36" t="s">
         <v>115</v>
       </c>
-      <c r="F42" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="G42" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="H42" s="37">
+      <c r="F42" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="G42" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="H42" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="35" t="s">
+      <c r="A43" s="36" t="s">
         <v>224</v>
       </c>
-      <c r="B43" s="36">
+      <c r="B43" s="37">
         <v>45311.0</v>
       </c>
-      <c r="C43" s="35" t="s">
+      <c r="C43" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="D43" s="35" t="s">
+      <c r="D43" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="E43" s="35" t="s">
+      <c r="E43" s="36" t="s">
         <v>127</v>
       </c>
-      <c r="F43" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="G43" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="H43" s="37">
+      <c r="F43" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="G43" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="H43" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="35" t="s">
+      <c r="A44" s="36" t="s">
         <v>225</v>
       </c>
-      <c r="B44" s="36">
+      <c r="B44" s="37">
         <v>45312.0</v>
       </c>
-      <c r="C44" s="35" t="s">
+      <c r="C44" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="D44" s="35" t="s">
+      <c r="D44" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="E44" s="35" t="s">
+      <c r="E44" s="36" t="s">
         <v>133</v>
       </c>
-      <c r="F44" s="35">
+      <c r="F44" s="36">
         <v>4.0</v>
       </c>
-      <c r="G44" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="H44" s="37">
+      <c r="G44" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="H44" s="38">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="35" t="s">
+      <c r="A45" s="36" t="s">
         <v>225</v>
       </c>
-      <c r="B45" s="36">
+      <c r="B45" s="37">
         <v>45312.0</v>
       </c>
-      <c r="C45" s="35" t="s">
+      <c r="C45" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="D45" s="35" t="s">
+      <c r="D45" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="E45" s="35" t="s">
+      <c r="E45" s="36" t="s">
         <v>121</v>
       </c>
-      <c r="F45" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="G45" s="35">
+      <c r="F45" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="G45" s="36">
         <v>4.0</v>
       </c>
-      <c r="H45" s="37">
+      <c r="H45" s="38">
         <f t="shared" si="1"/>
         <v>-4</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="35" t="s">
+      <c r="A46" s="36" t="s">
         <v>225</v>
       </c>
-      <c r="B46" s="36">
+      <c r="B46" s="37">
         <v>45312.0</v>
       </c>
-      <c r="C46" s="35" t="s">
+      <c r="C46" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="D46" s="35" t="s">
+      <c r="D46" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="E46" s="35" t="s">
+      <c r="E46" s="36" t="s">
         <v>140</v>
       </c>
-      <c r="F46" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="G46" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="H46" s="37">
+      <c r="F46" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="G46" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="H46" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="35" t="s">
+      <c r="A47" s="36" t="s">
         <v>225</v>
       </c>
-      <c r="B47" s="36">
+      <c r="B47" s="37">
         <v>45312.0</v>
       </c>
-      <c r="C47" s="35" t="s">
+      <c r="C47" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="D47" s="35" t="s">
+      <c r="D47" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="E47" s="35" t="s">
+      <c r="E47" s="36" t="s">
         <v>153</v>
       </c>
-      <c r="F47" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="G47" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="H47" s="37">
+      <c r="F47" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="G47" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="H47" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="35" t="s">
+      <c r="A48" s="36" t="s">
         <v>225</v>
       </c>
-      <c r="B48" s="36">
+      <c r="B48" s="37">
         <v>45312.0</v>
       </c>
-      <c r="C48" s="35" t="s">
+      <c r="C48" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="D48" s="35" t="s">
+      <c r="D48" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="E48" s="35" t="s">
+      <c r="E48" s="36" t="s">
         <v>159</v>
       </c>
-      <c r="F48" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="G48" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="H48" s="37">
+      <c r="F48" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="G48" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="H48" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="35" t="s">
+      <c r="A49" s="36" t="s">
         <v>225</v>
       </c>
-      <c r="B49" s="36">
+      <c r="B49" s="37">
         <v>45312.0</v>
       </c>
-      <c r="C49" s="35" t="s">
+      <c r="C49" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="D49" s="35" t="s">
+      <c r="D49" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="E49" s="35" t="s">
+      <c r="E49" s="36" t="s">
         <v>146</v>
       </c>
-      <c r="F49" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="G49" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="H49" s="37">
+      <c r="F49" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="G49" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="H49" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="35" t="s">
+      <c r="A50" s="36" t="s">
         <v>226</v>
       </c>
-      <c r="B50" s="36">
+      <c r="B50" s="37">
         <v>45313.0</v>
       </c>
-      <c r="C50" s="35" t="s">
+      <c r="C50" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="D50" s="35" t="s">
+      <c r="D50" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="E50" s="35" t="s">
+      <c r="E50" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="F50" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="G50" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="H50" s="37">
+      <c r="F50" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="G50" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="H50" s="38">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="35" t="s">
+      <c r="A51" s="36" t="s">
         <v>226</v>
       </c>
-      <c r="B51" s="36">
+      <c r="B51" s="37">
         <v>45313.0</v>
       </c>
-      <c r="C51" s="35" t="s">
+      <c r="C51" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="D51" s="35" t="s">
+      <c r="D51" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="E51" s="35" t="s">
+      <c r="E51" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="F51" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="G51" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="H51" s="37">
+      <c r="F51" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="G51" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="H51" s="38">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="35" t="s">
+      <c r="A52" s="36" t="s">
         <v>226</v>
       </c>
-      <c r="B52" s="36">
+      <c r="B52" s="37">
         <v>45313.0</v>
       </c>
-      <c r="C52" s="35" t="s">
+      <c r="C52" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="D52" s="35" t="s">
+      <c r="D52" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="E52" s="35" t="s">
+      <c r="E52" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="F52" s="35">
+      <c r="F52" s="36">
         <v>4.0</v>
       </c>
-      <c r="G52" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="H52" s="37">
+      <c r="G52" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="H52" s="38">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="35" t="s">
+      <c r="A53" s="36" t="s">
         <v>226</v>
       </c>
-      <c r="B53" s="36">
+      <c r="B53" s="37">
         <v>45313.0</v>
       </c>
-      <c r="C53" s="35" t="s">
+      <c r="C53" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="D53" s="35" t="s">
+      <c r="D53" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="E53" s="35" t="s">
+      <c r="E53" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="F53" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="G53" s="35">
+      <c r="F53" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="G53" s="36">
         <v>4.0</v>
       </c>
-      <c r="H53" s="37">
+      <c r="H53" s="38">
         <f t="shared" si="1"/>
         <v>-4</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="35" t="s">
+      <c r="A54" s="36" t="s">
         <v>226</v>
       </c>
-      <c r="B54" s="36">
+      <c r="B54" s="37">
         <v>45313.0</v>
       </c>
-      <c r="C54" s="35" t="s">
+      <c r="C54" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="D54" s="35" t="s">
+      <c r="D54" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="E54" s="35" t="s">
+      <c r="E54" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="F54" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="G54" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="H54" s="37">
+      <c r="F54" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="G54" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="H54" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="35" t="s">
+      <c r="A55" s="36" t="s">
         <v>226</v>
       </c>
-      <c r="B55" s="36">
+      <c r="B55" s="37">
         <v>45313.0</v>
       </c>
-      <c r="C55" s="35" t="s">
+      <c r="C55" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="D55" s="35" t="s">
+      <c r="D55" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="E55" s="35" t="s">
+      <c r="E55" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="F55" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="G55" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="H55" s="37">
+      <c r="F55" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="G55" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="H55" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="35" t="s">
+      <c r="A56" s="36" t="s">
         <v>226</v>
       </c>
-      <c r="B56" s="36">
+      <c r="B56" s="37">
         <v>45313.0</v>
       </c>
-      <c r="C56" s="35" t="s">
+      <c r="C56" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="D56" s="35" t="s">
+      <c r="D56" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="E56" s="35" t="s">
+      <c r="E56" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="F56" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="G56" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="H56" s="37">
+      <c r="F56" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="G56" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="H56" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="35" t="s">
+      <c r="A57" s="36" t="s">
         <v>226</v>
       </c>
-      <c r="B57" s="36">
+      <c r="B57" s="37">
         <v>45313.0</v>
       </c>
-      <c r="C57" s="35" t="s">
+      <c r="C57" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="D57" s="35" t="s">
+      <c r="D57" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="E57" s="35" t="s">
+      <c r="E57" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="F57" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="G57" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="H57" s="37">
+      <c r="F57" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="G57" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="H57" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="35" t="s">
+      <c r="A58" s="36" t="s">
         <v>227</v>
       </c>
-      <c r="B58" s="36">
+      <c r="B58" s="37">
         <v>45314.0</v>
       </c>
-      <c r="C58" s="35" t="s">
+      <c r="C58" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="D58" s="35" t="s">
+      <c r="D58" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="E58" s="35" t="s">
+      <c r="E58" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="F58" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="G58" s="35">
+      <c r="F58" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="G58" s="36">
         <v>3.0</v>
       </c>
-      <c r="H58" s="37">
+      <c r="H58" s="38">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="35" t="s">
+      <c r="A59" s="36" t="s">
         <v>227</v>
       </c>
-      <c r="B59" s="36">
+      <c r="B59" s="37">
         <v>45314.0</v>
       </c>
-      <c r="C59" s="35" t="s">
+      <c r="C59" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="D59" s="35" t="s">
+      <c r="D59" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="E59" s="35" t="s">
+      <c r="E59" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="F59" s="35">
+      <c r="F59" s="36">
         <v>3.0</v>
       </c>
-      <c r="G59" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="H59" s="37">
+      <c r="G59" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="H59" s="38">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="35" t="s">
+      <c r="A60" s="36" t="s">
         <v>227</v>
       </c>
-      <c r="B60" s="36">
+      <c r="B60" s="37">
         <v>45314.0</v>
       </c>
-      <c r="C60" s="35" t="s">
+      <c r="C60" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="D60" s="35" t="s">
+      <c r="D60" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="E60" s="35" t="s">
+      <c r="E60" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="F60" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="G60" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="H60" s="37">
+      <c r="F60" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="G60" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="H60" s="38">
         <f t="shared" si="1"/>
         <v>-2</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="35" t="s">
+      <c r="A61" s="36" t="s">
         <v>227</v>
       </c>
-      <c r="B61" s="36">
+      <c r="B61" s="37">
         <v>45314.0</v>
       </c>
-      <c r="C61" s="35" t="s">
+      <c r="C61" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="D61" s="35" t="s">
+      <c r="D61" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="E61" s="35" t="s">
+      <c r="E61" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="F61" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="G61" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="H61" s="37">
+      <c r="F61" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="G61" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="H61" s="38">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="35" t="s">
+      <c r="A62" s="36" t="s">
         <v>227</v>
       </c>
-      <c r="B62" s="36">
+      <c r="B62" s="37">
         <v>45314.0</v>
       </c>
-      <c r="C62" s="35" t="s">
+      <c r="C62" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="D62" s="35" t="s">
+      <c r="D62" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="E62" s="35" t="s">
+      <c r="E62" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="F62" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="G62" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="H62" s="37">
+      <c r="F62" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="G62" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="H62" s="38">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="35" t="s">
+      <c r="A63" s="36" t="s">
         <v>227</v>
       </c>
-      <c r="B63" s="36">
+      <c r="B63" s="37">
         <v>45314.0</v>
       </c>
-      <c r="C63" s="35" t="s">
+      <c r="C63" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="D63" s="35" t="s">
+      <c r="D63" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="E63" s="35" t="s">
+      <c r="E63" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="F63" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="G63" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="H63" s="37">
+      <c r="F63" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="G63" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="H63" s="38">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="35" t="s">
+      <c r="A64" s="36" t="s">
         <v>227</v>
       </c>
-      <c r="B64" s="36">
+      <c r="B64" s="37">
         <v>45314.0</v>
       </c>
-      <c r="C64" s="35" t="s">
+      <c r="C64" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="D64" s="35" t="s">
+      <c r="D64" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="E64" s="35" t="s">
+      <c r="E64" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="F64" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="G64" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="H64" s="37">
+      <c r="F64" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="G64" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="H64" s="38">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="35" t="s">
+      <c r="A65" s="36" t="s">
         <v>227</v>
       </c>
-      <c r="B65" s="36">
+      <c r="B65" s="37">
         <v>45314.0</v>
       </c>
-      <c r="C65" s="35" t="s">
+      <c r="C65" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="D65" s="35" t="s">
+      <c r="D65" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="E65" s="35" t="s">
+      <c r="E65" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="F65" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="G65" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="H65" s="37">
+      <c r="F65" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="G65" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="H65" s="38">
         <f t="shared" si="1"/>
         <v>-2</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="35" t="s">
+      <c r="A66" s="36" t="s">
         <v>228</v>
       </c>
-      <c r="B66" s="36">
+      <c r="B66" s="37">
         <v>45315.0</v>
       </c>
-      <c r="C66" s="35" t="s">
+      <c r="C66" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="D66" s="35" t="s">
+      <c r="D66" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="E66" s="35" t="s">
+      <c r="E66" s="36" t="s">
         <v>121</v>
       </c>
-      <c r="F66" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="G66" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="H66" s="37">
+      <c r="F66" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="G66" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="H66" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="35" t="s">
+      <c r="A67" s="36" t="s">
         <v>228</v>
       </c>
-      <c r="B67" s="36">
+      <c r="B67" s="37">
         <v>45315.0</v>
       </c>
-      <c r="C67" s="35" t="s">
+      <c r="C67" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="D67" s="35" t="s">
+      <c r="D67" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="E67" s="35" t="s">
+      <c r="E67" s="36" t="s">
         <v>127</v>
       </c>
-      <c r="F67" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="G67" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="H67" s="37">
+      <c r="F67" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="G67" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="H67" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="35" t="s">
+      <c r="A68" s="36" t="s">
         <v>228</v>
       </c>
-      <c r="B68" s="36">
+      <c r="B68" s="37">
         <v>45315.0</v>
       </c>
-      <c r="C68" s="35" t="s">
+      <c r="C68" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="D68" s="35" t="s">
+      <c r="D68" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="E68" s="35" t="s">
+      <c r="E68" s="36" t="s">
         <v>133</v>
       </c>
-      <c r="F68" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="G68" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="H68" s="37">
+      <c r="F68" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="G68" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="H68" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="35" t="s">
+      <c r="A69" s="36" t="s">
         <v>228</v>
       </c>
-      <c r="B69" s="36">
+      <c r="B69" s="37">
         <v>45315.0</v>
       </c>
-      <c r="C69" s="35" t="s">
+      <c r="C69" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="D69" s="35" t="s">
+      <c r="D69" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="E69" s="35" t="s">
+      <c r="E69" s="36" t="s">
         <v>115</v>
       </c>
-      <c r="F69" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="G69" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="H69" s="37">
+      <c r="F69" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="G69" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="H69" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="35" t="s">
+      <c r="A70" s="36" t="s">
         <v>228</v>
       </c>
-      <c r="B70" s="36">
+      <c r="B70" s="37">
         <v>45315.0</v>
       </c>
-      <c r="C70" s="35" t="s">
+      <c r="C70" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="D70" s="35" t="s">
+      <c r="D70" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="E70" s="35" t="s">
+      <c r="E70" s="36" t="s">
         <v>159</v>
       </c>
-      <c r="F70" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="G70" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="H70" s="37">
+      <c r="F70" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="G70" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="H70" s="38">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="35" t="s">
+      <c r="A71" s="36" t="s">
         <v>228</v>
       </c>
-      <c r="B71" s="36">
+      <c r="B71" s="37">
         <v>45315.0</v>
       </c>
-      <c r="C71" s="35" t="s">
+      <c r="C71" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="D71" s="35" t="s">
+      <c r="D71" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="E71" s="35" t="s">
+      <c r="E71" s="36" t="s">
         <v>140</v>
       </c>
-      <c r="F71" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="G71" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="H71" s="37">
+      <c r="F71" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="G71" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="H71" s="38">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="35" t="s">
+      <c r="A72" s="36" t="s">
         <v>228</v>
       </c>
-      <c r="B72" s="36">
+      <c r="B72" s="37">
         <v>45315.0</v>
       </c>
-      <c r="C72" s="35" t="s">
+      <c r="C72" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="D72" s="35" t="s">
+      <c r="D72" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="E72" s="35" t="s">
+      <c r="E72" s="36" t="s">
         <v>146</v>
       </c>
-      <c r="F72" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="G72" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="H72" s="37">
+      <c r="F72" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="G72" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="H72" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="35" t="s">
+      <c r="A73" s="36" t="s">
         <v>228</v>
       </c>
-      <c r="B73" s="36">
+      <c r="B73" s="37">
         <v>45315.0</v>
       </c>
-      <c r="C73" s="35" t="s">
+      <c r="C73" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="D73" s="35" t="s">
+      <c r="D73" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="E73" s="35" t="s">
+      <c r="E73" s="36" t="s">
         <v>153</v>
       </c>
-      <c r="F73" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="G73" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="H73" s="37">
+      <c r="F73" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="G73" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="H73" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="35" t="s">
+      <c r="A74" s="36" t="s">
         <v>229</v>
       </c>
-      <c r="B74" s="36">
+      <c r="B74" s="37">
         <v>45318.0</v>
       </c>
-      <c r="C74" s="35" t="s">
+      <c r="C74" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="D74" s="35" t="s">
+      <c r="D74" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="E74" s="35" t="s">
+      <c r="E74" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="F74" s="35">
+      <c r="F74" s="36">
         <v>3.0</v>
       </c>
-      <c r="G74" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="H74" s="37">
+      <c r="G74" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="H74" s="38">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="35" t="s">
+      <c r="A75" s="36" t="s">
         <v>229</v>
       </c>
-      <c r="B75" s="36">
+      <c r="B75" s="37">
         <v>45318.0</v>
       </c>
-      <c r="C75" s="35" t="s">
+      <c r="C75" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="D75" s="35" t="s">
+      <c r="D75" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="E75" s="35" t="s">
+      <c r="E75" s="36" t="s">
         <v>121</v>
       </c>
-      <c r="F75" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="G75" s="35">
+      <c r="F75" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="G75" s="36">
         <v>3.0</v>
       </c>
-      <c r="H75" s="37">
+      <c r="H75" s="38">
         <f t="shared" si="1"/>
         <v>-3</v>
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="35" t="s">
+      <c r="A76" s="36" t="s">
         <v>229</v>
       </c>
-      <c r="B76" s="36">
+      <c r="B76" s="37">
         <v>45318.0</v>
       </c>
-      <c r="C76" s="35" t="s">
+      <c r="C76" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="D76" s="35" t="s">
+      <c r="D76" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="E76" s="35" t="s">
+      <c r="E76" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="F76" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="G76" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="H76" s="37">
+      <c r="F76" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="G76" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="H76" s="38">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="35" t="s">
+      <c r="A77" s="36" t="s">
         <v>229</v>
       </c>
-      <c r="B77" s="36">
+      <c r="B77" s="37">
         <v>45318.0</v>
       </c>
-      <c r="C77" s="35" t="s">
+      <c r="C77" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="D77" s="35" t="s">
+      <c r="D77" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="E77" s="35" t="s">
+      <c r="E77" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="F77" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="G77" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="H77" s="37">
+      <c r="F77" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="G77" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="H77" s="38">
         <f t="shared" si="1"/>
         <v>-2</v>
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="35" t="s">
+      <c r="A78" s="36" t="s">
         <v>230</v>
       </c>
-      <c r="B78" s="36">
+      <c r="B78" s="37">
         <v>45319.0</v>
       </c>
-      <c r="C78" s="35" t="s">
+      <c r="C78" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="D78" s="35" t="s">
+      <c r="D78" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="E78" s="35" t="s">
+      <c r="E78" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="F78" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="G78" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="H78" s="37">
+      <c r="F78" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="G78" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="H78" s="38">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="35" t="s">
+      <c r="A79" s="36" t="s">
         <v>230</v>
       </c>
-      <c r="B79" s="36">
+      <c r="B79" s="37">
         <v>45319.0</v>
       </c>
-      <c r="C79" s="35" t="s">
+      <c r="C79" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="D79" s="35" t="s">
+      <c r="D79" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="E79" s="35" t="s">
+      <c r="E79" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="F79" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="G79" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="H79" s="37">
+      <c r="F79" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="G79" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="H79" s="38">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="35" t="s">
+      <c r="A80" s="36" t="s">
         <v>230</v>
       </c>
-      <c r="B80" s="36">
+      <c r="B80" s="37">
         <v>45319.0</v>
       </c>
-      <c r="C80" s="35" t="s">
+      <c r="C80" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="D80" s="35" t="s">
+      <c r="D80" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="E80" s="35" t="s">
+      <c r="E80" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="F80" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="G80" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="H80" s="37">
+      <c r="F80" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="G80" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="H80" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="35" t="s">
+      <c r="A81" s="36" t="s">
         <v>230</v>
       </c>
-      <c r="B81" s="36">
+      <c r="B81" s="37">
         <v>45319.0</v>
       </c>
-      <c r="C81" s="35" t="s">
+      <c r="C81" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="D81" s="35" t="s">
+      <c r="D81" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="E81" s="35" t="s">
+      <c r="E81" s="36" t="s">
         <v>153</v>
       </c>
-      <c r="F81" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="G81" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="H81" s="37">
+      <c r="F81" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="G81" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="H81" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="35" t="s">
+      <c r="A82" s="36" t="s">
         <v>231</v>
       </c>
-      <c r="B82" s="36">
+      <c r="B82" s="37">
         <v>45320.0</v>
       </c>
-      <c r="C82" s="35" t="s">
+      <c r="C82" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="D82" s="35" t="s">
+      <c r="D82" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="E82" s="35" t="s">
+      <c r="E82" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="F82" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="G82" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="H82" s="37">
+      <c r="F82" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="G82" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="H82" s="38">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="35" t="s">
+      <c r="A83" s="36" t="s">
         <v>231</v>
       </c>
-      <c r="B83" s="36">
+      <c r="B83" s="37">
         <v>45320.0</v>
       </c>
-      <c r="C83" s="35" t="s">
+      <c r="C83" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="D83" s="35" t="s">
+      <c r="D83" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="E83" s="35" t="s">
+      <c r="E83" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="F83" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="G83" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="H83" s="37">
+      <c r="F83" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="G83" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="H83" s="38">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="35" t="s">
+      <c r="A84" s="36" t="s">
         <v>231</v>
       </c>
-      <c r="B84" s="36">
+      <c r="B84" s="37">
         <v>45320.0</v>
       </c>
-      <c r="C84" s="35" t="s">
+      <c r="C84" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="D84" s="35" t="s">
+      <c r="D84" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="E84" s="35" t="s">
+      <c r="E84" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="F84" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="G84" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="H84" s="37">
+      <c r="F84" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="G84" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="H84" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="35" t="s">
+      <c r="A85" s="36" t="s">
         <v>231</v>
       </c>
-      <c r="B85" s="36">
+      <c r="B85" s="37">
         <v>45320.0</v>
       </c>
-      <c r="C85" s="35" t="s">
+      <c r="C85" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="D85" s="35" t="s">
+      <c r="D85" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="E85" s="35" t="s">
+      <c r="E85" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="F85" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="G85" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="H85" s="37">
+      <c r="F85" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="G85" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="H85" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="35" t="s">
+      <c r="A86" s="36" t="s">
         <v>232</v>
       </c>
-      <c r="B86" s="36">
+      <c r="B86" s="37">
         <v>45321.0</v>
       </c>
-      <c r="C86" s="35" t="s">
+      <c r="C86" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="D86" s="35" t="s">
+      <c r="D86" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="E86" s="35" t="s">
+      <c r="E86" s="36" t="s">
         <v>127</v>
       </c>
-      <c r="F86" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="G86" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="H86" s="37">
+      <c r="F86" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="G86" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="H86" s="38">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="35" t="s">
+      <c r="A87" s="36" t="s">
         <v>232</v>
       </c>
-      <c r="B87" s="36">
+      <c r="B87" s="37">
         <v>45321.0</v>
       </c>
-      <c r="C87" s="35" t="s">
+      <c r="C87" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="D87" s="35" t="s">
+      <c r="D87" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="E87" s="35" t="s">
+      <c r="E87" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="F87" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="G87" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="H87" s="37">
+      <c r="F87" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="G87" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="H87" s="38">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="35" t="s">
+      <c r="A88" s="36" t="s">
         <v>232</v>
       </c>
-      <c r="B88" s="36">
+      <c r="B88" s="37">
         <v>45321.0</v>
       </c>
-      <c r="C88" s="35" t="s">
+      <c r="C88" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="D88" s="35" t="s">
+      <c r="D88" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="E88" s="35" t="s">
+      <c r="E88" s="36" t="s">
         <v>140</v>
       </c>
-      <c r="F88" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="G88" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="H88" s="37">
+      <c r="F88" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="G88" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="H88" s="38">
         <f t="shared" si="1"/>
         <v>-2</v>
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="35" t="s">
+      <c r="A89" s="36" t="s">
         <v>232</v>
       </c>
-      <c r="B89" s="36">
+      <c r="B89" s="37">
         <v>45321.0</v>
       </c>
-      <c r="C89" s="35" t="s">
+      <c r="C89" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="D89" s="35" t="s">
+      <c r="D89" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="E89" s="35" t="s">
+      <c r="E89" s="36" t="s">
         <v>133</v>
       </c>
-      <c r="F89" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="G89" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="H89" s="37">
+      <c r="F89" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="G89" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="H89" s="38">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="35" t="s">
+      <c r="A90" s="36" t="s">
         <v>233</v>
       </c>
-      <c r="B90" s="36">
+      <c r="B90" s="37">
         <v>45324.0</v>
       </c>
-      <c r="C90" s="35" t="s">
+      <c r="C90" s="36" t="s">
         <v>183</v>
       </c>
-      <c r="D90" s="35" t="s">
+      <c r="D90" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="E90" s="35" t="s">
+      <c r="E90" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="F90" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="G90" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="H90" s="37">
+      <c r="F90" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="G90" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="H90" s="38">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="35" t="s">
+      <c r="A91" s="36" t="s">
         <v>233</v>
       </c>
-      <c r="B91" s="36">
+      <c r="B91" s="37">
         <v>45324.0</v>
       </c>
-      <c r="C91" s="35" t="s">
+      <c r="C91" s="36" t="s">
         <v>183</v>
       </c>
-      <c r="D91" s="35" t="s">
+      <c r="D91" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="E91" s="35" t="s">
+      <c r="E91" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="F91" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="G91" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="H91" s="37">
+      <c r="F91" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="G91" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="H91" s="38">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="35" t="s">
+      <c r="A92" s="36" t="s">
         <v>233</v>
       </c>
-      <c r="B92" s="36">
+      <c r="B92" s="37">
         <v>45324.0</v>
       </c>
-      <c r="C92" s="35" t="s">
+      <c r="C92" s="36" t="s">
         <v>183</v>
       </c>
-      <c r="D92" s="35" t="s">
+      <c r="D92" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="E92" s="35" t="s">
+      <c r="E92" s="36" t="s">
         <v>153</v>
       </c>
-      <c r="F92" s="35">
+      <c r="F92" s="36">
         <v>3.0</v>
       </c>
-      <c r="G92" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="H92" s="37">
+      <c r="G92" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="H92" s="38">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="35" t="s">
+      <c r="A93" s="36" t="s">
         <v>233</v>
       </c>
-      <c r="B93" s="36">
+      <c r="B93" s="37">
         <v>45324.0</v>
       </c>
-      <c r="C93" s="35" t="s">
+      <c r="C93" s="36" t="s">
         <v>183</v>
       </c>
-      <c r="D93" s="35" t="s">
+      <c r="D93" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="E93" s="35" t="s">
+      <c r="E93" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="F93" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="G93" s="35">
+      <c r="F93" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="G93" s="36">
         <v>3.0</v>
       </c>
-      <c r="H93" s="37">
+      <c r="H93" s="38">
         <f t="shared" si="1"/>
         <v>-2</v>
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="35" t="s">
+      <c r="A94" s="36" t="s">
         <v>234</v>
       </c>
-      <c r="B94" s="36">
+      <c r="B94" s="37">
         <v>45325.0</v>
       </c>
-      <c r="C94" s="35" t="s">
+      <c r="C94" s="36" t="s">
         <v>183</v>
       </c>
-      <c r="D94" s="35" t="s">
+      <c r="D94" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="E94" s="35" t="s">
+      <c r="E94" s="36" t="s">
         <v>127</v>
       </c>
-      <c r="F94" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="G94" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="H94" s="37">
+      <c r="F94" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="G94" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="H94" s="38">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="35" t="s">
+      <c r="A95" s="36" t="s">
         <v>234</v>
       </c>
-      <c r="B95" s="36">
+      <c r="B95" s="37">
         <v>45325.0</v>
       </c>
-      <c r="C95" s="35" t="s">
+      <c r="C95" s="36" t="s">
         <v>183</v>
       </c>
-      <c r="D95" s="35" t="s">
+      <c r="D95" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="E95" s="35" t="s">
+      <c r="E95" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="F95" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="G95" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="H95" s="37">
+      <c r="F95" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="G95" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="H95" s="38">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="35" t="s">
+      <c r="A96" s="36" t="s">
         <v>234</v>
       </c>
-      <c r="B96" s="36">
+      <c r="B96" s="37">
         <v>45325.0</v>
       </c>
-      <c r="C96" s="35" t="s">
+      <c r="C96" s="36" t="s">
         <v>183</v>
       </c>
-      <c r="D96" s="35" t="s">
+      <c r="D96" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="E96" s="35" t="s">
+      <c r="E96" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="F96" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="G96" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="H96" s="37">
+      <c r="F96" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="G96" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="H96" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="35" t="s">
+      <c r="A97" s="36" t="s">
         <v>234</v>
       </c>
-      <c r="B97" s="36">
+      <c r="B97" s="37">
         <v>45325.0</v>
       </c>
-      <c r="C97" s="35" t="s">
+      <c r="C97" s="36" t="s">
         <v>183</v>
       </c>
-      <c r="D97" s="35" t="s">
+      <c r="D97" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="E97" s="35" t="s">
+      <c r="E97" s="36" t="s">
         <v>133</v>
       </c>
-      <c r="F97" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="G97" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="H97" s="37">
+      <c r="F97" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="G97" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="H97" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="35" t="s">
+      <c r="A98" s="36" t="s">
         <v>235</v>
       </c>
-      <c r="B98" s="36">
+      <c r="B98" s="37">
         <v>45329.0</v>
       </c>
-      <c r="C98" s="35" t="s">
+      <c r="C98" s="36" t="s">
         <v>184</v>
       </c>
-      <c r="D98" s="35" t="s">
+      <c r="D98" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="E98" s="35" t="s">
+      <c r="E98" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="F98" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="G98" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="H98" s="37">
+      <c r="F98" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="G98" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="H98" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="35" t="s">
+      <c r="A99" s="36" t="s">
         <v>235</v>
       </c>
-      <c r="B99" s="36">
+      <c r="B99" s="37">
         <v>45329.0</v>
       </c>
-      <c r="C99" s="35" t="s">
+      <c r="C99" s="36" t="s">
         <v>184</v>
       </c>
-      <c r="D99" s="35" t="s">
+      <c r="D99" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="E99" s="35" t="s">
+      <c r="E99" s="36" t="s">
         <v>133</v>
       </c>
-      <c r="F99" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="G99" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="H99" s="37">
+      <c r="F99" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="G99" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="H99" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="35" t="s">
+      <c r="A100" s="36" t="s">
         <v>235</v>
       </c>
-      <c r="B100" s="36">
+      <c r="B100" s="37">
         <v>45329.0</v>
       </c>
-      <c r="C100" s="35" t="s">
+      <c r="C100" s="36" t="s">
         <v>184</v>
       </c>
-      <c r="D100" s="35" t="s">
+      <c r="D100" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="E100" s="35" t="s">
+      <c r="E100" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="F100" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="G100" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="H100" s="37">
+      <c r="F100" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="G100" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="H100" s="38">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="35" t="s">
+      <c r="A101" s="36" t="s">
         <v>235</v>
       </c>
-      <c r="B101" s="36">
+      <c r="B101" s="37">
         <v>45329.0</v>
       </c>
-      <c r="C101" s="35" t="s">
+      <c r="C101" s="36" t="s">
         <v>184</v>
       </c>
-      <c r="D101" s="35" t="s">
+      <c r="D101" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="E101" s="35" t="s">
+      <c r="E101" s="36" t="s">
         <v>153</v>
       </c>
-      <c r="F101" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="G101" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="H101" s="37">
+      <c r="F101" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="G101" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="H101" s="38">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="35" t="s">
+      <c r="A102" s="36" t="s">
         <v>236</v>
       </c>
-      <c r="B102" s="36">
+      <c r="B102" s="37">
         <v>45332.0</v>
       </c>
-      <c r="C102" s="35" t="s">
+      <c r="C102" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="D102" s="35" t="s">
+      <c r="D102" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="E102" s="35" t="s">
+      <c r="E102" s="36" t="s">
         <v>133</v>
       </c>
-      <c r="F102" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="G102" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="H102" s="37">
+      <c r="F102" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="G102" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="H102" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="35" t="s">
+      <c r="A103" s="36" t="s">
         <v>236</v>
       </c>
-      <c r="B103" s="36">
+      <c r="B103" s="37">
         <v>45332.0</v>
       </c>
-      <c r="C103" s="35" t="s">
+      <c r="C103" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="D103" s="35" t="s">
+      <c r="D103" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="E103" s="35" t="s">
+      <c r="E103" s="36" t="s">
         <v>153</v>
       </c>
-      <c r="F103" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="G103" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="H103" s="37">
+      <c r="F103" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="G103" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="H103" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="35" t="s">
+      <c r="A104" s="36" t="s">
         <v>237</v>
       </c>
-      <c r="B104" s="36">
+      <c r="B104" s="37">
         <v>45333.0</v>
       </c>
-      <c r="C104" s="35" t="s">
+      <c r="C104" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="D104" s="35" t="s">
+      <c r="D104" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="E104" s="35" t="s">
+      <c r="E104" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="F104" s="37"/>
-      <c r="G104" s="37"/>
-      <c r="H104" s="37">
+      <c r="F104" s="38"/>
+      <c r="G104" s="38"/>
+      <c r="H104" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="35" t="s">
+      <c r="A105" s="36" t="s">
         <v>237</v>
       </c>
-      <c r="B105" s="36">
+      <c r="B105" s="37">
         <v>45333.0</v>
       </c>
-      <c r="C105" s="35" t="s">
+      <c r="C105" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="D105" s="35" t="s">
+      <c r="D105" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="E105" s="35" t="s">
+      <c r="E105" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="F105" s="37"/>
-      <c r="G105" s="37"/>
-      <c r="H105" s="37">
+      <c r="F105" s="38"/>
+      <c r="G105" s="38"/>
+      <c r="H105" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -18492,98 +18645,98 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="36" t="s">
         <v>330</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="39" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="36" t="s">
         <v>332</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="36" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="36" t="s">
         <v>334</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="36" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="36" t="s">
         <v>336</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="36" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="36" t="s">
         <v>338</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="36" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="36" t="s">
         <v>340</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="36" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="36" t="s">
         <v>342</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="36" t="s">
         <v>343</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="36" t="s">
         <v>344</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="36" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="36" t="s">
         <v>346</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="36" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="36" t="s">
         <v>348</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="36" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="36" t="s">
         <v>349</v>
       </c>
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="36" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="36" t="s">
         <v>351</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="36" t="s">
         <v>352</v>
       </c>
     </row>
@@ -18625,7 +18778,7 @@
       <c r="B2" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="36" t="s">
         <v>339</v>
       </c>
     </row>
@@ -18636,7 +18789,7 @@
       <c r="B3" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="C3" s="37"/>
+      <c r="C3" s="38"/>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
@@ -18645,7 +18798,7 @@
       <c r="B4" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="C4" s="37"/>
+      <c r="C4" s="38"/>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
@@ -18654,7 +18807,7 @@
       <c r="B5" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="C5" s="37"/>
+      <c r="C5" s="38"/>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
@@ -18663,7 +18816,7 @@
       <c r="B6" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="C6" s="37"/>
+      <c r="C6" s="38"/>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
@@ -18672,7 +18825,7 @@
       <c r="B7" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="C7" s="37"/>
+      <c r="C7" s="38"/>
     </row>
     <row r="8">
       <c r="A8" s="6" t="s">
@@ -18681,7 +18834,7 @@
       <c r="B8" s="6" t="s">
         <v>356</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="36" t="s">
         <v>341</v>
       </c>
     </row>
@@ -18692,7 +18845,7 @@
       <c r="B9" s="6" t="s">
         <v>356</v>
       </c>
-      <c r="C9" s="37"/>
+      <c r="C9" s="38"/>
     </row>
     <row r="10">
       <c r="A10" s="6" t="s">
@@ -18701,7 +18854,7 @@
       <c r="B10" s="6" t="s">
         <v>356</v>
       </c>
-      <c r="C10" s="37"/>
+      <c r="C10" s="38"/>
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
@@ -18710,7 +18863,7 @@
       <c r="B11" s="6" t="s">
         <v>356</v>
       </c>
-      <c r="C11" s="37"/>
+      <c r="C11" s="38"/>
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
@@ -18719,7 +18872,7 @@
       <c r="B12" s="6" t="s">
         <v>356</v>
       </c>
-      <c r="C12" s="37"/>
+      <c r="C12" s="38"/>
     </row>
     <row r="13">
       <c r="A13" s="6" t="s">
@@ -18728,7 +18881,7 @@
       <c r="B13" s="6" t="s">
         <v>356</v>
       </c>
-      <c r="C13" s="37"/>
+      <c r="C13" s="38"/>
     </row>
     <row r="14">
       <c r="A14" s="8" t="s">
@@ -18737,7 +18890,7 @@
       <c r="B14" s="8" t="s">
         <v>358</v>
       </c>
-      <c r="C14" s="37"/>
+      <c r="C14" s="38"/>
     </row>
     <row r="15">
       <c r="A15" s="8" t="s">
@@ -18746,7 +18899,7 @@
       <c r="B15" s="8" t="s">
         <v>358</v>
       </c>
-      <c r="C15" s="37"/>
+      <c r="C15" s="38"/>
     </row>
     <row r="16">
       <c r="A16" s="8" t="s">
@@ -18755,7 +18908,7 @@
       <c r="B16" s="8" t="s">
         <v>358</v>
       </c>
-      <c r="C16" s="37"/>
+      <c r="C16" s="38"/>
     </row>
     <row r="17">
       <c r="A17" s="8" t="s">
@@ -18764,7 +18917,7 @@
       <c r="B17" s="8" t="s">
         <v>358</v>
       </c>
-      <c r="C17" s="37"/>
+      <c r="C17" s="38"/>
     </row>
     <row r="18">
       <c r="A18" s="8" t="s">
@@ -18773,7 +18926,7 @@
       <c r="B18" s="8" t="s">
         <v>358</v>
       </c>
-      <c r="C18" s="37"/>
+      <c r="C18" s="38"/>
     </row>
     <row r="19">
       <c r="A19" s="8" t="s">
@@ -18782,7 +18935,7 @@
       <c r="B19" s="8" t="s">
         <v>358</v>
       </c>
-      <c r="C19" s="37"/>
+      <c r="C19" s="38"/>
     </row>
     <row r="20">
       <c r="A20" s="8" t="s">
@@ -18791,7 +18944,7 @@
       <c r="B20" s="8" t="s">
         <v>358</v>
       </c>
-      <c r="C20" s="37"/>
+      <c r="C20" s="38"/>
     </row>
     <row r="21">
       <c r="A21" s="31" t="s">
@@ -18800,7 +18953,7 @@
       <c r="B21" s="31" t="s">
         <v>359</v>
       </c>
-      <c r="C21" s="37"/>
+      <c r="C21" s="38"/>
     </row>
     <row r="22">
       <c r="A22" s="31" t="s">
@@ -18809,7 +18962,7 @@
       <c r="B22" s="31" t="s">
         <v>359</v>
       </c>
-      <c r="C22" s="37"/>
+      <c r="C22" s="38"/>
     </row>
     <row r="23">
       <c r="A23" s="31" t="s">
@@ -18818,7 +18971,7 @@
       <c r="B23" s="31" t="s">
         <v>359</v>
       </c>
-      <c r="C23" s="37"/>
+      <c r="C23" s="38"/>
     </row>
     <row r="24">
       <c r="A24" s="10" t="s">
@@ -18854,10 +19007,10 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="39" t="s">
+      <c r="A27" s="27" t="s">
         <v>213</v>
       </c>
-      <c r="B27" s="39" t="s">
+      <c r="B27" s="27" t="s">
         <v>362</v>
       </c>
       <c r="C27" s="40"/>
@@ -24619,13 +24772,13 @@
       <c r="S103" s="54"/>
     </row>
     <row r="104">
-      <c r="A104" s="55">
+      <c r="A104" s="28">
         <v>45333.0</v>
       </c>
-      <c r="B104" s="39" t="s">
+      <c r="B104" s="27" t="s">
         <v>397</v>
       </c>
-      <c r="C104" s="39" t="s">
+      <c r="C104" s="27" t="s">
         <v>181</v>
       </c>
       <c r="D104" s="40"/>
@@ -24646,13 +24799,13 @@
       <c r="S104" s="40"/>
     </row>
     <row r="105">
-      <c r="A105" s="55">
+      <c r="A105" s="28">
         <v>45333.0</v>
       </c>
-      <c r="B105" s="39" t="s">
+      <c r="B105" s="27" t="s">
         <v>397</v>
       </c>
-      <c r="C105" s="39" t="s">
+      <c r="C105" s="27" t="s">
         <v>181</v>
       </c>
       <c r="D105" s="40"/>

</xml_diff>